<commit_message>
2, 3 changes with diplaying mean rather than regularization
</commit_message>
<xml_diff>
--- a/static/graphs/data.xlsx
+++ b/static/graphs/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B214"/>
+  <dimension ref="A1:B272"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2014,173 +2014,629 @@
       </c>
     </row>
     <row r="198">
-      <c r="A198" t="inlineStr">
-        <is>
-          <t>20230203</t>
-        </is>
+      <c r="A198" t="n">
+        <v>20230203</v>
       </c>
       <c r="B198" t="n">
         <v>1.271000057458878</v>
       </c>
     </row>
     <row r="199">
-      <c r="A199" t="inlineStr">
-        <is>
-          <t>20230208</t>
-        </is>
+      <c r="A199" t="n">
+        <v>20230208</v>
       </c>
       <c r="B199" t="n">
         <v>1.316999942064285</v>
       </c>
     </row>
     <row r="200">
-      <c r="A200" t="inlineStr">
-        <is>
-          <t>20230213</t>
-        </is>
+      <c r="A200" t="n">
+        <v>20230213</v>
       </c>
       <c r="B200" t="n">
         <v>1.324999928474426</v>
       </c>
     </row>
     <row r="201">
-      <c r="A201" t="inlineStr">
-        <is>
-          <t>20230218</t>
-        </is>
+      <c r="A201" t="n">
+        <v>20230218</v>
       </c>
       <c r="B201" t="n">
         <v>1.309999972581863</v>
       </c>
     </row>
     <row r="202">
-      <c r="A202" t="inlineStr">
-        <is>
-          <t>20230223</t>
-        </is>
+      <c r="A202" t="n">
+        <v>20230223</v>
       </c>
       <c r="B202" t="n">
         <v>1.313000023365021</v>
       </c>
     </row>
     <row r="203">
-      <c r="A203" t="inlineStr">
-        <is>
-          <t>20230228</t>
-        </is>
+      <c r="A203" t="n">
+        <v>20230228</v>
       </c>
       <c r="B203" t="n">
         <v>1.574999988079071</v>
       </c>
     </row>
     <row r="204">
-      <c r="A204" t="inlineStr">
+      <c r="A204" t="n">
+        <v>20230305</v>
+      </c>
+      <c r="B204" t="n">
+        <v>1.771000027656555</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>20230310</v>
+      </c>
+      <c r="B205" t="n">
+        <v>1.615999937057495</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>20230315</v>
+      </c>
+      <c r="B206" t="n">
+        <v>3.242000043392181</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>20230320</v>
+      </c>
+      <c r="B207" t="n">
+        <v>1.307000070810318</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>20230325</v>
+      </c>
+      <c r="B208" t="n">
+        <v>1.301999986171722</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>20230330</v>
+      </c>
+      <c r="B209" t="n">
+        <v>1.342000067234039</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>20230404</v>
+      </c>
+      <c r="B210" t="n">
+        <v>1.456999927759171</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>20230409</v>
+      </c>
+      <c r="B211" t="n">
+        <v>1.335999965667725</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>20230414</v>
+      </c>
+      <c r="B212" t="n">
+        <v>1.270000040531158</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>20230419</v>
+      </c>
+      <c r="B213" t="n">
+        <v>1.488000005483627</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>20230424</v>
+      </c>
+      <c r="B214" t="n">
+        <v>1.666000038385391</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>20230305</v>
+      </c>
+      <c r="B215" t="n">
+        <v>1.780000030994415</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="n">
+        <v>20230310</v>
+      </c>
+      <c r="B216" t="n">
+        <v>1.573999971151352</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>20230315</v>
+      </c>
+      <c r="B217" t="n">
+        <v>1.544999927282333</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="n">
+        <v>20230320</v>
+      </c>
+      <c r="B218" t="n">
+        <v>1.334999948740005</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="n">
+        <v>20230325</v>
+      </c>
+      <c r="B219" t="n">
+        <v>1.272000074386597</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>20230330</v>
+      </c>
+      <c r="B220" t="n">
+        <v>1.389999985694885</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>20230404</v>
+      </c>
+      <c r="B221" t="n">
+        <v>1.402000039815903</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>20230409</v>
+      </c>
+      <c r="B222" t="n">
+        <v>1.372999995946884</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>20230414</v>
+      </c>
+      <c r="B223" t="n">
+        <v>1.272999942302704</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="n">
+        <v>20230419</v>
+      </c>
+      <c r="B224" t="n">
+        <v>1.500999927520752</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="n">
+        <v>20230424</v>
+      </c>
+      <c r="B225" t="n">
+        <v>1.405999958515167</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>20230429</v>
+      </c>
+      <c r="B226" t="n">
+        <v>1.928000003099442</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="n">
+        <v>20230504</v>
+      </c>
+      <c r="B227" t="n">
+        <v>1.22299998998642</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="n">
+        <v>20230305</v>
+      </c>
+      <c r="B228" t="n">
+        <v>1.790000051259995</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="n">
+        <v>20230310</v>
+      </c>
+      <c r="B229" t="n">
+        <v>1.60300001502037</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="n">
+        <v>20230315</v>
+      </c>
+      <c r="B230" t="n">
+        <v>1.198000013828278</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="n">
+        <v>20230320</v>
+      </c>
+      <c r="B231" t="n">
+        <v>1.319999992847443</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="n">
+        <v>20230325</v>
+      </c>
+      <c r="B232" t="n">
+        <v>1.269000023603439</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="n">
+        <v>20230330</v>
+      </c>
+      <c r="B233" t="n">
+        <v>1.331000030040741</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="n">
+        <v>20230404</v>
+      </c>
+      <c r="B234" t="n">
+        <v>1.397999972105026</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="n">
+        <v>20230409</v>
+      </c>
+      <c r="B235" t="n">
+        <v>1.442999988794327</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="n">
+        <v>20230414</v>
+      </c>
+      <c r="B236" t="n">
+        <v>1.308999955654144</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>20230419</v>
+      </c>
+      <c r="B237" t="n">
+        <v>1.474000066518784</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>20230424</v>
+      </c>
+      <c r="B238" t="n">
+        <v>1.430000066757202</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>20230429</v>
+      </c>
+      <c r="B239" t="n">
+        <v>1.668000072240829</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>20230504</v>
+      </c>
+      <c r="B240" t="n">
+        <v>1.234999969601631</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="n">
+        <v>20230305</v>
+      </c>
+      <c r="B241" t="n">
+        <v>1.816000044345856</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="n">
+        <v>20230310</v>
+      </c>
+      <c r="B242" t="n">
+        <v>1.553999930620193</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="n">
+        <v>20230315</v>
+      </c>
+      <c r="B243" t="n">
+        <v>1.407999992370605</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="n">
+        <v>20230320</v>
+      </c>
+      <c r="B244" t="n">
+        <v>1.337999999523163</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="n">
+        <v>20230325</v>
+      </c>
+      <c r="B245" t="n">
+        <v>1.180000007152557</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="n">
+        <v>20230330</v>
+      </c>
+      <c r="B246" t="n">
+        <v>1.221000030636787</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="n">
+        <v>20230404</v>
+      </c>
+      <c r="B247" t="n">
+        <v>1.292999982833862</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="n">
+        <v>20230409</v>
+      </c>
+      <c r="B248" t="n">
+        <v>1.381999999284744</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="n">
+        <v>20230414</v>
+      </c>
+      <c r="B249" t="n">
+        <v>1.289999932050705</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="n">
+        <v>20230419</v>
+      </c>
+      <c r="B250" t="n">
+        <v>1.381999999284744</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="n">
+        <v>20230424</v>
+      </c>
+      <c r="B251" t="n">
+        <v>1.29600003361702</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="n">
+        <v>20230429</v>
+      </c>
+      <c r="B252" t="n">
+        <v>6.155999898910522</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="n">
+        <v>20230504</v>
+      </c>
+      <c r="B253" t="n">
+        <v>1.142999976873398</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="n">
+        <v>20220608</v>
+      </c>
+      <c r="B254" t="n">
+        <v>8.059999942779541</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="n">
+        <v>20220613</v>
+      </c>
+      <c r="B255" t="n">
+        <v>8.672000169754028</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="n">
+        <v>20220618</v>
+      </c>
+      <c r="B256" t="n">
+        <v>1.951999962329865</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="n">
+        <v>20220703</v>
+      </c>
+      <c r="B257" t="n">
+        <v>8.880000114440918</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="n">
+        <v>20220901</v>
+      </c>
+      <c r="B258" t="n">
+        <v>1.578000038862228</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="n">
+        <v>20220906</v>
+      </c>
+      <c r="B259" t="n">
+        <v>1.159000024199486</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
         <is>
           <t>20230305</t>
         </is>
       </c>
-      <c r="B204" t="n">
-        <v>1.771000027656555</v>
-      </c>
-    </row>
-    <row r="205">
-      <c r="A205" t="inlineStr">
+      <c r="B260" t="n">
+        <v>1.781000047922134</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
         <is>
           <t>20230310</t>
         </is>
       </c>
-      <c r="B205" t="n">
-        <v>1.615999937057495</v>
-      </c>
-    </row>
-    <row r="206">
-      <c r="A206" t="inlineStr">
+      <c r="B261" t="n">
+        <v>1.596000045537949</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
         <is>
           <t>20230315</t>
         </is>
       </c>
-      <c r="B206" t="n">
-        <v>3.242000043392181</v>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" t="inlineStr">
+      <c r="B262" t="n">
+        <v>1.757999956607819</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
         <is>
           <t>20230320</t>
         </is>
       </c>
-      <c r="B207" t="n">
-        <v>1.307000070810318</v>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" t="inlineStr">
+      <c r="B263" t="n">
+        <v>1.31400004029274</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
         <is>
           <t>20230325</t>
         </is>
       </c>
-      <c r="B208" t="n">
-        <v>1.301999986171722</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" t="inlineStr">
+      <c r="B264" t="n">
+        <v>1.274999976158142</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
         <is>
           <t>20230330</t>
         </is>
       </c>
-      <c r="B209" t="n">
-        <v>1.342000067234039</v>
-      </c>
-    </row>
-    <row r="210">
-      <c r="A210" t="inlineStr">
+      <c r="B265" t="n">
+        <v>1.425999999046326</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
         <is>
           <t>20230404</t>
         </is>
       </c>
-      <c r="B210" t="n">
-        <v>1.456999927759171</v>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" t="inlineStr">
+      <c r="B266" t="n">
+        <v>1.421000063419342</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
         <is>
           <t>20230409</t>
         </is>
       </c>
-      <c r="B211" t="n">
-        <v>1.335999965667725</v>
-      </c>
-    </row>
-    <row r="212">
-      <c r="A212" t="inlineStr">
+      <c r="B267" t="n">
+        <v>1.333999931812286</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
         <is>
           <t>20230414</t>
         </is>
       </c>
-      <c r="B212" t="n">
-        <v>1.270000040531158</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" t="inlineStr">
+      <c r="B268" t="n">
+        <v>1.27700001001358</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
         <is>
           <t>20230419</t>
         </is>
       </c>
-      <c r="B213" t="n">
-        <v>1.488000005483627</v>
-      </c>
-    </row>
-    <row r="214">
-      <c r="A214" t="inlineStr">
+      <c r="B269" t="n">
+        <v>1.480000019073486</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
         <is>
           <t>20230424</t>
         </is>
       </c>
-      <c r="B214" t="n">
-        <v>1.666000038385391</v>
+      <c r="B270" t="n">
+        <v>1.440999954938889</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>20230429</t>
+        </is>
+      </c>
+      <c r="B271" t="n">
+        <v>1.867000013589859</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>20230504</t>
+        </is>
+      </c>
+      <c r="B272" t="n">
+        <v>1.24600000679493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>